<commit_message>
navigation and narrative changes
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-PADI-Provenance.xlsx
+++ b/output/StructureDefinition-PADI-Provenance.xlsx
@@ -689,7 +689,7 @@
     <t>Provenance.agent.who</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner|PractitionerRole|RelatedPerson|http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient|Device|http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization)
+    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner|http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient|http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization)
 </t>
   </si>
   <si>
@@ -728,7 +728,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-provenance-1:onBehalfOf SHALL be present when Provenance.agent.who is a Practitioner or Device {($this.agent.who.resolve().is Practitioner or Device) implies exists()}</t>
+provenance-1:onBehalfOf SHALL be present when Provenance.agent.who is a Practitioner or Device {(($this.agent.who.resolve() is Practitioner) or ($this.agent.who.resolve() is Device)) implies exists()}</t>
   </si>
   <si>
     <t>Person, Practitioner, Organization, Device :* .role [classCode = RoleClassMutualRelationship; role.code and * .scopes[Role](classCode=IDENT) and *.plays [Role.Code]</t>

</xml_diff>